<commit_message>
add 4 code clinic from file excel - 03.03.2023
</commit_message>
<xml_diff>
--- a/uploads/(Formatted)-20230116 Clinics - VN - Latest 16.01.23 copy.xlsx
+++ b/uploads/(Formatted)-20230116 Clinics - VN - Latest 16.01.23 copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michace/Desktop/SAS/tools/sas-export-clinics-from-excel/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45353F3B-186D-AD41-8D7E-71EF5BB3745F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF78D16E-8870-6240-88CF-0B14174390FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" xr2:uid="{CD5FCDE9-40CA-A645-8A7E-D71150EC814D}"/>
+    <workbookView xWindow="45700" yWindow="2740" windowWidth="34560" windowHeight="20340" xr2:uid="{CD5FCDE9-40CA-A645-8A7E-D71150EC814D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6969" uniqueCount="3338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7051" uniqueCount="3375">
   <si>
     <t>Tiếng Việt</t>
   </si>
@@ -10213,12 +10213,123 @@
   <si>
     <t>1 Ton That Tung, Dong Da District, Ha Noi</t>
   </si>
+  <si>
+    <t>PKDKJHTB</t>
+  </si>
+  <si>
+    <t>Phòng khám Đa khoa Jio Health Tân Bình</t>
+  </si>
+  <si>
+    <t>Tầng trệt tòa nhà Republic Plaza, số 18E Cộng Hòa, Phường 4</t>
+  </si>
+  <si>
+    <t>Thứ 2 - Chủ nhật: 07:00 - 20:00</t>
+  </si>
+  <si>
+    <t>Jio Health Polyclinic Tan Binh</t>
+  </si>
+  <si>
+    <t>Ground Floor Republic Plaza, No.18E Cong Hoa, Ward 4</t>
+  </si>
+  <si>
+    <t>Mon– Sun: 07:00 - 20:00</t>
+  </si>
+  <si>
+    <t>Tầng trệt tòa nhà Republic Plaza, số 18E Cộng Hòa, Phường 4, Quận Tân Bình, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Ground Floor Republic Plaza, No.18E Cong Hoa,Ward 4 Tan Binh District Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>PKDKJHTD</t>
+  </si>
+  <si>
+    <t>Phòng khám Đa khoa Jio Health Thảo Điền</t>
+  </si>
+  <si>
+    <t>Tầng trệt – Tầng 3 – Tầng 4 Tòa nhà Worc@Q2, số 21 Võ Trường Toản, Phường Thảo Điền</t>
+  </si>
+  <si>
+    <t>Jio Health Polyclinic Thao Dien</t>
+  </si>
+  <si>
+    <t>Ground Floor – 3rd Floor – 4th Floor, Worc@Q2 Building, No. 21 Vo Truong Toan, Thao Dien Ward</t>
+  </si>
+  <si>
+    <t>Tầng trệt – Tầng 3 – Tầng 4 Tòa nhà Worc@Q2, số 21 Võ Trường Toản, Phường Thảo Điền, TP Thủ Đức Thu Duc City</t>
+  </si>
+  <si>
+    <t>Ground Floor – 3rd Floor – 4th Floor,Worc@Q2 Building, No. 21 Vo Truong Toan,Thao Dien Ward Thu Duc City Thu Duc City</t>
+  </si>
+  <si>
+    <t>PKDKJHBD</t>
+  </si>
+  <si>
+    <t>Phòng khám Đa khoa Jio Health Ba Đình</t>
+  </si>
+  <si>
+    <t>Tầng B1, Capital Place, 29 Liễu Giai, Ngọc Khánh</t>
+  </si>
+  <si>
+    <t>Jio Health Polyclinic Ba Dinh</t>
+  </si>
+  <si>
+    <t>Floor B1, Capital Place, 29 Lieu Giai, Ngoc Khanh</t>
+  </si>
+  <si>
+    <t>Tầng B1, Capital Place, 29 Liễu Giai, Ngọc Khánh, Quận Ba Đình, Hà Nội</t>
+  </si>
+  <si>
+    <t>Floor B1, Capital Place, 29 Lieu Giai, Ngoc Khanh Ba Dinh District Ha Noi</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>BV175</t>
+  </si>
+  <si>
+    <t>Bệnh Viện Quân Y 175</t>
+  </si>
+  <si>
+    <t>786 Nguyễn Kiệm, Phường 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">028 62 89 03 57    </t>
+  </si>
+  <si>
+    <t>Thứ 2 - Thứ 6: 08:00 - 16:00</t>
+  </si>
+  <si>
+    <t>Hiện tại BV chưa tiếp nhận BLVP với SAS do quy trình nội bộ</t>
+  </si>
+  <si>
+    <t>Melitary Hospital 175</t>
+  </si>
+  <si>
+    <t>786 Nguyen Kiem, Ward 3</t>
+  </si>
+  <si>
+    <t>Mon - Friday: 08:00 - 16:00</t>
+  </si>
+  <si>
+    <t>No provide directbilling services due to internal procedure</t>
+  </si>
+  <si>
+    <t>https://benhvien175.vn/</t>
+  </si>
+  <si>
+    <t>786 Nguyễn Kiệm, Phường 3, Quận Gò Vấp, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>786 Nguyen Kiem, Ward 3 Go Vap District Ho Chi Minh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10351,6 +10462,13 @@
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -10616,7 +10734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -10962,6 +11080,24 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -10986,23 +11122,38 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12037,10 +12188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3996FE01-6E8E-7E4B-AF8A-2F606D870DA8}">
-  <dimension ref="A1:AD271"/>
+  <dimension ref="A1:AE275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z180" zoomScale="92" workbookViewId="0">
-      <selection activeCell="Z184" sqref="Z184"/>
+    <sheetView tabSelected="1" topLeftCell="A260" zoomScale="92" workbookViewId="0">
+      <selection activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12083,38 +12234,38 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="119" t="s">
+      <c r="J1" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="119"/>
-      <c r="P1" s="119"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="125"/>
       <c r="Q1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="120" t="s">
+      <c r="R1" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="120"/>
-      <c r="T1" s="120"/>
-      <c r="U1" s="121" t="s">
+      <c r="S1" s="126"/>
+      <c r="T1" s="126"/>
+      <c r="U1" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="121"/>
-      <c r="W1" s="122" t="s">
+      <c r="V1" s="127"/>
+      <c r="W1" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="123"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="125" t="s">
+      <c r="X1" s="129"/>
+      <c r="Y1" s="130"/>
+      <c r="Z1" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="AA1" s="126"/>
+      <c r="AA1" s="132"/>
     </row>
-    <row r="2" spans="1:29" ht="140" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="154" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -34560,7 +34711,7 @@
       </c>
     </row>
     <row r="271" spans="1:30" ht="28" x14ac:dyDescent="0.2">
-      <c r="A271" s="127" t="s">
+      <c r="A271" s="119" t="s">
         <v>3326</v>
       </c>
       <c r="B271" s="101" t="s">
@@ -34575,13 +34726,13 @@
       <c r="E271" s="110" t="s">
         <v>60</v>
       </c>
-      <c r="F271" s="127">
+      <c r="F271" s="119">
         <v>19006422</v>
       </c>
       <c r="G271" s="105" t="s">
         <v>3329</v>
       </c>
-      <c r="H271" s="128" t="s">
+      <c r="H271" s="120" t="s">
         <v>3330</v>
       </c>
       <c r="I271" s="106" t="s">
@@ -34608,31 +34759,31 @@
       <c r="P271" s="106" t="s">
         <v>69</v>
       </c>
-      <c r="Q271" s="129" t="s">
+      <c r="Q271" s="121" t="s">
         <v>3335</v>
       </c>
-      <c r="R271" s="130"/>
-      <c r="S271" s="130" t="s">
-        <v>51</v>
-      </c>
-      <c r="T271" s="130" t="s">
-        <v>51</v>
-      </c>
-      <c r="U271" s="131" t="s">
-        <v>51</v>
-      </c>
-      <c r="V271" s="131"/>
-      <c r="W271" s="132">
+      <c r="R271" s="122"/>
+      <c r="S271" s="122" t="s">
+        <v>51</v>
+      </c>
+      <c r="T271" s="122" t="s">
+        <v>51</v>
+      </c>
+      <c r="U271" s="123" t="s">
+        <v>51</v>
+      </c>
+      <c r="V271" s="123"/>
+      <c r="W271" s="124">
         <v>21.002674580000001</v>
       </c>
-      <c r="X271" s="132">
+      <c r="X271" s="124">
         <v>105.83025379999999</v>
       </c>
-      <c r="Y271" s="132"/>
-      <c r="Z271" s="130" t="s">
+      <c r="Y271" s="124"/>
+      <c r="Z271" s="122" t="s">
         <v>3336</v>
       </c>
-      <c r="AA271" s="131" t="s">
+      <c r="AA271" s="123" t="s">
         <v>3337</v>
       </c>
       <c r="AB271" s="115" t="s">
@@ -34642,6 +34793,323 @@
         <v>32</v>
       </c>
       <c r="AD271" s="20"/>
+    </row>
+    <row r="272" spans="1:30" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A272" s="100" t="s">
+        <v>3338</v>
+      </c>
+      <c r="B272" s="101" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C272" s="86" t="s">
+        <v>3339</v>
+      </c>
+      <c r="D272" s="112" t="s">
+        <v>3340</v>
+      </c>
+      <c r="E272" s="110" t="s">
+        <v>775</v>
+      </c>
+      <c r="F272" s="104">
+        <v>1900636893</v>
+      </c>
+      <c r="G272" s="105" t="s">
+        <v>3341</v>
+      </c>
+      <c r="H272" s="92"/>
+      <c r="I272" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="J272" s="88" t="s">
+        <v>3342</v>
+      </c>
+      <c r="K272" s="105" t="s">
+        <v>3343</v>
+      </c>
+      <c r="L272" s="99" t="s">
+        <v>779</v>
+      </c>
+      <c r="M272" s="103">
+        <v>1900636893</v>
+      </c>
+      <c r="N272" s="105" t="s">
+        <v>3344</v>
+      </c>
+      <c r="O272" s="98"/>
+      <c r="P272" s="106" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q272" s="107" t="s">
+        <v>3047</v>
+      </c>
+      <c r="R272" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="S272" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="T272" s="133"/>
+      <c r="U272" s="133"/>
+      <c r="V272" s="133"/>
+      <c r="W272" s="28">
+        <v>10.8033940385126</v>
+      </c>
+      <c r="X272" s="28">
+        <v>106.655155089914</v>
+      </c>
+      <c r="Y272" s="28"/>
+      <c r="Z272" s="112" t="s">
+        <v>3345</v>
+      </c>
+      <c r="AA272" s="112" t="s">
+        <v>3346</v>
+      </c>
+      <c r="AB272" s="115" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC272" s="115" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="273" spans="1:31" ht="34" x14ac:dyDescent="0.2">
+      <c r="A273" s="100" t="s">
+        <v>3347</v>
+      </c>
+      <c r="B273" s="101" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C273" s="86" t="s">
+        <v>3348</v>
+      </c>
+      <c r="D273" s="112" t="s">
+        <v>3349</v>
+      </c>
+      <c r="E273" s="110" t="s">
+        <v>2439</v>
+      </c>
+      <c r="F273" s="104">
+        <v>1900636893</v>
+      </c>
+      <c r="G273" s="105" t="s">
+        <v>3341</v>
+      </c>
+      <c r="H273" s="92"/>
+      <c r="I273" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="J273" s="88" t="s">
+        <v>3350</v>
+      </c>
+      <c r="K273" s="105" t="s">
+        <v>3351</v>
+      </c>
+      <c r="L273" s="99" t="s">
+        <v>2443</v>
+      </c>
+      <c r="M273" s="103">
+        <v>1900636893</v>
+      </c>
+      <c r="N273" s="105" t="s">
+        <v>3344</v>
+      </c>
+      <c r="O273" s="98"/>
+      <c r="P273" s="106" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q273" s="107" t="s">
+        <v>3047</v>
+      </c>
+      <c r="R273" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="S273" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="T273" s="133"/>
+      <c r="U273" s="133"/>
+      <c r="V273" s="133"/>
+      <c r="W273" s="28">
+        <v>10.806147372626199</v>
+      </c>
+      <c r="X273" s="28">
+        <v>106.746978475538</v>
+      </c>
+      <c r="Y273" s="28"/>
+      <c r="Z273" s="112" t="s">
+        <v>3352</v>
+      </c>
+      <c r="AA273" s="112" t="s">
+        <v>3353</v>
+      </c>
+      <c r="AB273" s="115" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC273" s="115" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="274" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A274" s="118" t="s">
+        <v>3354</v>
+      </c>
+      <c r="B274" s="134" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C274" s="80" t="s">
+        <v>3355</v>
+      </c>
+      <c r="D274" s="135" t="s">
+        <v>3356</v>
+      </c>
+      <c r="E274" s="136" t="s">
+        <v>214</v>
+      </c>
+      <c r="F274" s="137">
+        <v>1900636893</v>
+      </c>
+      <c r="G274" s="138" t="s">
+        <v>3341</v>
+      </c>
+      <c r="H274" s="96"/>
+      <c r="I274" s="139" t="s">
+        <v>63</v>
+      </c>
+      <c r="J274" s="83" t="s">
+        <v>3357</v>
+      </c>
+      <c r="K274" s="138" t="s">
+        <v>3358</v>
+      </c>
+      <c r="L274" s="140" t="s">
+        <v>219</v>
+      </c>
+      <c r="M274" s="141">
+        <v>1900636893</v>
+      </c>
+      <c r="N274" s="138" t="s">
+        <v>3344</v>
+      </c>
+      <c r="O274" s="142"/>
+      <c r="P274" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q274" s="143" t="s">
+        <v>3047</v>
+      </c>
+      <c r="R274" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="S274" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="T274" s="133"/>
+      <c r="U274" s="133"/>
+      <c r="V274" s="133"/>
+      <c r="W274" s="28">
+        <v>21.031300230512599</v>
+      </c>
+      <c r="X274" s="62">
+        <v>105.81361113225999</v>
+      </c>
+      <c r="Y274" s="28"/>
+      <c r="Z274" s="112" t="s">
+        <v>3359</v>
+      </c>
+      <c r="AA274" s="112" t="s">
+        <v>3360</v>
+      </c>
+      <c r="AB274" s="115" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC274" s="115" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE274" t="s">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="275" spans="1:31" ht="17" x14ac:dyDescent="0.2">
+      <c r="A275" s="118" t="s">
+        <v>3362</v>
+      </c>
+      <c r="B275" s="134" t="s">
+        <v>37</v>
+      </c>
+      <c r="C275" s="80" t="s">
+        <v>3363</v>
+      </c>
+      <c r="D275" s="135" t="s">
+        <v>3364</v>
+      </c>
+      <c r="E275" s="136" t="s">
+        <v>228</v>
+      </c>
+      <c r="F275" s="137" t="s">
+        <v>3365</v>
+      </c>
+      <c r="G275" s="138" t="s">
+        <v>3366</v>
+      </c>
+      <c r="H275" s="96" t="s">
+        <v>3367</v>
+      </c>
+      <c r="I275" s="139" t="s">
+        <v>43</v>
+      </c>
+      <c r="J275" s="83" t="s">
+        <v>3368</v>
+      </c>
+      <c r="K275" s="138" t="s">
+        <v>3369</v>
+      </c>
+      <c r="L275" s="140" t="s">
+        <v>233</v>
+      </c>
+      <c r="M275" s="141" t="s">
+        <v>3365</v>
+      </c>
+      <c r="N275" s="138" t="s">
+        <v>3370</v>
+      </c>
+      <c r="O275" s="142" t="s">
+        <v>3371</v>
+      </c>
+      <c r="P275" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q275" s="143" t="s">
+        <v>3372</v>
+      </c>
+      <c r="R275" s="133"/>
+      <c r="S275" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="T275" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="U275" s="133" t="s">
+        <v>51</v>
+      </c>
+      <c r="V275" s="133"/>
+      <c r="W275" s="28">
+        <v>10.820034856568199</v>
+      </c>
+      <c r="X275" s="62">
+        <v>106.679930774501</v>
+      </c>
+      <c r="Y275" s="28"/>
+      <c r="Z275" s="112" t="s">
+        <v>3373</v>
+      </c>
+      <c r="AA275" s="112" t="s">
+        <v>3374</v>
+      </c>
+      <c r="AB275" s="115" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC275" s="115" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>